<commit_message>
MD5 einer Datei effizient berechnen
</commit_message>
<xml_diff>
--- a/createDB/Datebmodell.xlsx
+++ b/createDB/Datebmodell.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\KOST\workbench\TiffAnalyseProject\createDB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tools\Gowork\src\github.com\KOST-CECO\TiffAnalyseProject\createDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Tabelle1!$A$1:$E$37</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Tabelle1!$A$1:$E$39</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="70">
   <si>
     <t>name</t>
   </si>
@@ -226,6 +226,18 @@
   </si>
   <si>
     <t>Zeitpunkt und Flag für den Abschluss der Analyse</t>
+  </si>
+  <si>
+    <t>mimetype</t>
+  </si>
+  <si>
+    <t>Internet Media Type, auch MIME-Type aufgrund der Magic Number</t>
+  </si>
+  <si>
+    <t>filesize</t>
+  </si>
+  <si>
+    <t>Dateigrösse in Byte</t>
   </si>
 </sst>
 </file>
@@ -787,10 +799,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -942,7 +954,7 @@
         <v>49</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>10</v>
@@ -972,7 +984,7 @@
         <v>52</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>12</v>
@@ -981,353 +993,383 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
       <c r="B13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="5"/>
+      <c r="B14" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="6" t="s">
+      <c r="D14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8" t="s">
+    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C15" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="9" t="s">
+      <c r="D15" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="4" t="s">
+      <c r="C18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
-      <c r="B17" s="1" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="5"/>
+      <c r="B19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" s="6" t="s">
+      <c r="C19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="5"/>
-      <c r="B18" s="1" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="5"/>
+      <c r="B20" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" s="6" t="s">
+      <c r="D20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8" t="s">
+    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C21" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19" s="9" t="s">
+      <c r="D21" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21" s="4" t="s">
+      <c r="D23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
-      <c r="B22" s="1" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="5"/>
+      <c r="B24" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" s="6" t="s">
+      <c r="D24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="8" t="s">
+    <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C25" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E23" s="9" t="s">
+      <c r="D25" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+    <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="15"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E27" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="5"/>
-      <c r="B26" s="1" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="5"/>
+      <c r="B28" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E26" s="6" t="s">
+      <c r="C28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="5"/>
-      <c r="B27" s="1" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="5"/>
+      <c r="B29" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E27" s="6" t="s">
+      <c r="C29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="8" t="s">
+    <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E28" s="9" t="s">
+      <c r="C30" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E30" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+    <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="15"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B32" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E30" s="4" t="s">
+      <c r="C32" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="5"/>
-      <c r="B31" s="1" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="5"/>
+      <c r="B33" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E31" s="6" t="s">
+      <c r="C33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E33" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="8" t="s">
+    <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="7"/>
+      <c r="B34" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E32" s="9" t="s">
+      <c r="C34" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E34" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
+    <row r="35" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="15"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E34" s="6" t="s">
+      <c r="C36" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E36" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="5"/>
-      <c r="B35" s="1" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="5"/>
+      <c r="B37" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E35" s="6" t="s">
+      <c r="C37" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E37" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="5"/>
-      <c r="B36" s="1" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="5"/>
+      <c r="B38" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E36" s="6" t="s">
+      <c r="D38" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E38" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
-      <c r="B37" s="8" t="s">
+    <row r="39" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="7"/>
+      <c r="B39" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C39" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D37" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E37" s="9" t="s">
+      <c r="D39" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E39" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B40" s="13"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="13"/>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B42" s="13"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>